<commit_message>
2nd content organization commit
</commit_message>
<xml_diff>
--- a/logHours.xlsx
+++ b/logHours.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Cheers Cut Log Book</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t xml:space="preserve">Doing some content </t>
+  </si>
+  <si>
+    <t>Imported Graphics 1</t>
+  </si>
+  <si>
+    <t>Fixed DNS issue WTF GoDaddy, and set up social media accounts, talked to Bomyee abt shit</t>
   </si>
 </sst>
 </file>
@@ -104,12 +110,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -414,7 +423,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,18 +505,36 @@
       <c r="A6" s="2">
         <v>42514</v>
       </c>
-      <c r="D6">
-        <f>Table1[[#This Row],[Clocik-out]]-Table1[[#This Row],[Clock-in]]</f>
-        <v>0</v>
+      <c r="B6" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D6" s="3">
+        <f>Table1[[#This Row],[Clocik-out]]-Table1[[#This Row],[Clock-in]]</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>42515</v>
       </c>
-      <c r="D7">
-        <f>Table1[[#This Row],[Clocik-out]]-Table1[[#This Row],[Clock-in]]</f>
-        <v>0</v>
+      <c r="B7" s="4">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.9375</v>
+      </c>
+      <c r="D7" s="3">
+        <f>Table1[[#This Row],[Clocik-out]]-Table1[[#This Row],[Clock-in]]</f>
+        <v>0.20833333333333337</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>